<commit_message>
Add - formula to 'contracted in *month*'
</commit_message>
<xml_diff>
--- a/data/input/Transactions.xlsx
+++ b/data/input/Transactions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biacarvalheira/Desktop/excelWebScript/data/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biacarvalheira/Desktop/DEVELOPMENT/FREELANCER/excelWeb_script/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC8480B-9ED4-D141-8089-9C007D23CA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ED3059-9187-A043-B10D-E708DED6B112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{A15CC418-AF70-D545-BBFE-8CB1E831B78D}"/>
   </bookViews>
@@ -518,7 +518,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,7 +698,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>45273</v>
+        <v>45182</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="4" t="s">
@@ -776,7 +776,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>45273</v>
+        <v>44939</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="4" t="s">

</xml_diff>